<commit_message>
Minor Cleanups / Mapping Concept for Body Slave
</commit_message>
<xml_diff>
--- a/docs/Port Mapping.xlsx
+++ b/docs/Port Mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nobser/Projects/GitHub/BetterDuinoFirmwareV4/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7ADCE4-9499-3B48-B5A8-E6A5D9D992E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F783122D-8BAE-9046-99A1-F19FCB393C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11480" yWindow="7100" windowWidth="35280" windowHeight="18660" xr2:uid="{4F6A979C-00BB-A740-AF26-7BB99DEBB3CB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
   <si>
     <t>Dome Master</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>Function</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>AltFunc</t>
   </si>
 </sst>
 </file>
@@ -485,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B623611-0137-C84F-8B2F-0C99999D714F}">
-  <dimension ref="A3:S13"/>
+  <dimension ref="A3:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23:J24"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -932,6 +938,50 @@
         <v>23</v>
       </c>
     </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>14</v>
+      </c>
+      <c r="F14">
+        <v>15</v>
+      </c>
+      <c r="G14">
+        <v>16</v>
+      </c>
+      <c r="H14">
+        <v>17</v>
+      </c>
+      <c r="I14">
+        <v>18</v>
+      </c>
+      <c r="J14">
+        <v>19</v>
+      </c>
+      <c r="K14">
+        <v>20</v>
+      </c>
+      <c r="L14">
+        <v>21</v>
+      </c>
+      <c r="M14">
+        <v>22</v>
+      </c>
+      <c r="R14" t="s">
+        <v>29</v>
+      </c>
+      <c r="S14" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>